<commit_message>
changed variable behavior, now its real $vars
</commit_message>
<xml_diff>
--- a/beispiel.xlsx
+++ b/beispiel.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t xml:space="preserve">erg</t>
   </si>
@@ -34,6 +34,9 @@
     <t xml:space="preserve">Phy</t>
   </si>
   <si>
+    <t xml:space="preserve">more</t>
+  </si>
+  <si>
     <t xml:space="preserve">!U/I </t>
   </si>
   <si>
@@ -50,6 +53,12 @@
   </si>
   <si>
     <t xml:space="preserve">Die fette alte wiegt $val1 kg und trägt noch eine tasche mit sich die $val2 kg wiegt. Wie schwer ist die Alte wenn die mit der Tasche in der hand auf der waage steht. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">!F*G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Das hier nen test $F(3,6) mal $G(2,5)</t>
   </si>
   <si>
     <t xml:space="preserve">!U**2/R </t>
@@ -199,16 +208,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="31.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="44.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="39.97"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -230,46 +240,58 @@
       <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="48.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="196.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="104.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -277,10 +299,10 @@
     </row>
     <row r="5" customFormat="false" ht="69.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -288,10 +310,10 @@
     </row>
     <row r="6" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>

</xml_diff>

<commit_message>
removed annoying ! from calc field
</commit_message>
<xml_diff>
--- a/beispiel.xlsx
+++ b/beispiel.xlsx
@@ -37,46 +37,46 @@
     <t xml:space="preserve">more</t>
   </si>
   <si>
-    <t xml:space="preserve">!U/I </t>
+    <t xml:space="preserve">U/I </t>
   </si>
   <si>
     <t xml:space="preserve">Bei einer Eingeschalteten Lampe wird ein Strom von $I A gemessen. An der Lampe liegen $U V an. Wie groß ist der Widerstand ?</t>
   </si>
   <si>
-    <t xml:space="preserve">!Fr(2,val1)+Fr(val3,val2) </t>
+    <t xml:space="preserve">Fr(2,val1)+Fr(val3,val2) </t>
   </si>
   <si>
     <t xml:space="preserve">$ \frac{2}{$val1} + \frac{$val3}{$val2} $</t>
   </si>
   <si>
-    <t xml:space="preserve">!val1+val2 </t>
+    <t xml:space="preserve">val1+val2 </t>
   </si>
   <si>
     <t xml:space="preserve">Die fette alte wiegt $val1 kg und trägt noch eine tasche mit sich die $val2 kg wiegt. Wie schwer ist die Alte wenn die mit der Tasche in der hand auf der waage steht. </t>
   </si>
   <si>
-    <t xml:space="preserve">!F*G</t>
+    <t xml:space="preserve">F*G</t>
   </si>
   <si>
     <t xml:space="preserve">Das hier nen test $F(3,6) mal $G(2,5)</t>
   </si>
   <si>
-    <t xml:space="preserve">!U**2/R </t>
+    <t xml:space="preserve">U**2/R </t>
   </si>
   <si>
     <t xml:space="preserve">Eine lose Klemme hat einen Übergangwiderstand von etwa $R Ohm bei einer Spannung von $U V. Welche Leistung entsteht hier? </t>
   </si>
   <si>
-    <t xml:space="preserve">["Ein Quadrat hat eine Seiten länge von $val1 cm", ["!val1*4", "Wie groß ist der Umfang"], ["!val1**2", "Wie groß ist die Fläche"], ["!val2*4","Wie groß wäre der Umfang, wenn die Seitenlänge $val2 cm wäre."]] </t>
-  </si>
-  <si>
-    <t xml:space="preserve">!R*I </t>
+    <t xml:space="preserve">["Ein Quadrat hat eine Seiten länge von $val1 cm", ["val1*4", "Wie groß ist der Umfang"], ["val1**2", "Wie groß ist die Fläche"], ["val2*4","Wie groß wäre der Umfang, wenn die Seitenlänge $val2 cm wäre."]] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R*I </t>
   </si>
   <si>
     <t xml:space="preserve">Ein elektrischer Heizlüfter hat einen Widerstand von $R $ \Omega $ und belastet die Leitung mit $I A. Welche elektrische Spannung wird benötigt, um den Heizlüfter zu betreiben? </t>
   </si>
   <si>
-    <t xml:space="preserve">!U/(R*1000) </t>
+    <t xml:space="preserve">U/(R*1000) </t>
   </si>
   <si>
     <t xml:space="preserve">In einem experimentellen Schaltkreis beträgt der Widerstand $R kOhm und die angelegte elektrische Spannung entspricht $U V . Wie groß ist die Stromstärke, die durch den Schaltkreis fließt? </t>
@@ -211,7 +211,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
fix a problem with variables
</commit_message>
<xml_diff>
--- a/beispiel.xlsx
+++ b/beispiel.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t xml:space="preserve">erg</t>
   </si>
@@ -68,6 +68,12 @@
   </si>
   <si>
     <t xml:space="preserve">["Ein Quadrat hat eine Seiten länge von $val1 cm", ["val1*4", "Wie groß ist der Umfang"], ["val1**2", "Wie groß ist die Fläche"], ["val2*4","Wie groß wäre der Umfang, wenn die Seitenlänge $val2 cm wäre."]] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(e*m)/Temp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Das $m(2,23) kg schwere schiff lädt $e(3,7) Kisten bei $Temp(25,30) °C auf.</t>
   </si>
   <si>
     <t xml:space="preserve">R*I </t>
@@ -210,8 +216,8 @@
   </sheetPr>
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -284,14 +290,19 @@
       <c r="D3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="5"/>
+      <c r="E3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -299,10 +310,10 @@
     </row>
     <row r="5" customFormat="false" ht="69.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -310,10 +321,10 @@
     </row>
     <row r="6" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>

</xml_diff>